<commit_message>
fix conversation, update doccument
</commit_message>
<xml_diff>
--- a/server/documents/api/HTTP_API.xlsx
+++ b/server/documents/api/HTTP_API.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="10"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="get_nonce" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="login" sheetId="4" r:id="rId3"/>
     <sheet name="upload single" sheetId="6" r:id="rId4"/>
     <sheet name="upload multiple" sheetId="7" r:id="rId5"/>
-    <sheet name="user info" sheetId="9" r:id="rId6"/>
-    <sheet name="messages" sheetId="11" r:id="rId7"/>
-    <sheet name="settings" sheetId="12" r:id="rId8"/>
-    <sheet name="location" sheetId="13" r:id="rId9"/>
-    <sheet name="get swipes" sheetId="14" r:id="rId10"/>
-    <sheet name="converstions" sheetId="15" r:id="rId11"/>
-    <sheet name="delete_image" sheetId="17" r:id="rId12"/>
+    <sheet name="get_image" sheetId="19" r:id="rId6"/>
+    <sheet name="user info" sheetId="9" r:id="rId7"/>
+    <sheet name="messages" sheetId="11" r:id="rId8"/>
+    <sheet name="settings" sheetId="12" r:id="rId9"/>
+    <sheet name="location" sheetId="13" r:id="rId10"/>
+    <sheet name="get swipes" sheetId="14" r:id="rId11"/>
+    <sheet name="converstions" sheetId="15" r:id="rId12"/>
+    <sheet name="delete_image" sheetId="17" r:id="rId13"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="165">
   <si>
     <t>Project</t>
   </si>
@@ -635,6 +636,30 @@
   </si>
   <si>
     <t>Body</t>
+  </si>
+  <si>
+    <t>/upload/${user_id}_image${num}.jpg</t>
+  </si>
+  <si>
+    <t>http://localhost:3000/upload/1_image2.jpg</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>&lt;image data&gt;</t>
+  </si>
+  <si>
+    <t>Internal Server Error 400</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> { "message": "File not found." }</t>
+  </si>
+  <si>
+    <t>Download user profile image</t>
+  </si>
+  <si>
+    <t>get_image</t>
   </si>
 </sst>
 </file>
@@ -1103,7 +1128,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="142">
+  <cellXfs count="144">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1384,6 +1409,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1426,6 +1454,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1441,6 +1475,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1450,17 +1487,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1769,7 +1800,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1821,48 +1852,48 @@
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="122"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="123"/>
     </row>
     <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="122" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="123"/>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="125"/>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="126" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="127"/>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="118" t="s">
+      <c r="A8" s="119" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -1879,14 +1910,14 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="101.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="119"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="13"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="120"/>
+      <c r="A10" s="121"/>
       <c r="B10" s="5"/>
       <c r="C10" s="13"/>
       <c r="D10" s="14"/>
@@ -1904,7 +1935,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="117" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="15"/>
@@ -1913,7 +1944,7 @@
       <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:5" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="117"/>
+      <c r="A13" s="118"/>
       <c r="B13" s="18"/>
       <c r="C13" s="21" t="s">
         <v>21</v>
@@ -1940,6 +1971,243 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="59.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>43575</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="139" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="123"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="139" t="s">
+        <v>130</v>
+      </c>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="123"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="140" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="125"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="126" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="127"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="119" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="120"/>
+      <c r="B9" s="84" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="86" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="86">
+        <v>10.8770936</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="133"/>
+      <c r="B10" s="93" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="100" t="s">
+        <v>133</v>
+      </c>
+      <c r="D10" s="105">
+        <v>106.8032315</v>
+      </c>
+      <c r="E10" s="86"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="75"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="B12" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="77" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="61" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="22"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" s="16"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="117" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="13"/>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="134"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="88" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" s="65"/>
+      <c r="F15" s="66"/>
+    </row>
+    <row r="16" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="134"/>
+      <c r="B16" s="113"/>
+      <c r="C16" s="90" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="89" t="s">
+        <v>136</v>
+      </c>
+      <c r="E16" s="30"/>
+      <c r="F16" s="25"/>
+    </row>
+    <row r="17" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="118"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="76" t="s">
+        <v>78</v>
+      </c>
+      <c r="E17" s="73"/>
+      <c r="F17" s="74"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A8:A10"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -1986,49 +2254,49 @@
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="139" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="122"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="135" t="s">
+      <c r="B5" s="139" t="s">
         <v>139</v>
       </c>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="136" t="s">
+      <c r="B6" s="140" t="s">
         <v>140</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="125"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="127"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="50" t="s">
@@ -2087,7 +2355,7 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="117" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="15"/>
@@ -2097,7 +2365,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="288.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="131"/>
+      <c r="A13" s="134"/>
       <c r="B13" s="33"/>
       <c r="C13" s="63" t="s">
         <v>76</v>
@@ -2109,7 +2377,7 @@
       <c r="F13" s="66"/>
     </row>
     <row r="14" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="131"/>
+      <c r="A14" s="134"/>
       <c r="B14" s="113"/>
       <c r="C14" s="90" t="s">
         <v>83</v>
@@ -2121,7 +2389,7 @@
       <c r="F14" s="25"/>
     </row>
     <row r="15" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="117"/>
+      <c r="A15" s="118"/>
       <c r="B15" s="18"/>
       <c r="C15" s="115" t="s">
         <v>49</v>
@@ -2147,11 +2415,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -2194,49 +2462,49 @@
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="139" t="s">
         <v>145</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="122"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="135" t="s">
+      <c r="B5" s="139" t="s">
         <v>147</v>
       </c>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="136" t="s">
+      <c r="B6" s="140" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="125"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="127"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="52" t="s">
@@ -2295,7 +2563,7 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="117" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="15"/>
@@ -2305,7 +2573,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="409.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="131"/>
+      <c r="A13" s="134"/>
       <c r="B13" s="33"/>
       <c r="C13" s="63" t="s">
         <v>76</v>
@@ -2317,7 +2585,7 @@
       <c r="F13" s="66"/>
     </row>
     <row r="14" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="117"/>
+      <c r="A14" s="118"/>
       <c r="B14" s="18"/>
       <c r="C14" s="115" t="s">
         <v>49</v>
@@ -2343,7 +2611,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
@@ -2390,52 +2658,52 @@
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="122" t="s">
         <v>150</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="122"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="122" t="s">
         <v>151</v>
       </c>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>152</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="125"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="127"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="132" t="s">
+      <c r="A8" s="135" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -2455,7 +2723,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="133"/>
+      <c r="A9" s="136"/>
       <c r="B9" s="5" t="s">
         <v>70</v>
       </c>
@@ -2469,7 +2737,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="134"/>
+      <c r="A10" s="137"/>
       <c r="B10" s="16"/>
       <c r="C10" s="4"/>
       <c r="D10" s="57"/>
@@ -2505,7 +2773,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="117" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="15"/>
@@ -2515,7 +2783,7 @@
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="131"/>
+      <c r="A14" s="134"/>
       <c r="B14" s="33"/>
       <c r="C14" s="63" t="s">
         <v>76</v>
@@ -2527,7 +2795,7 @@
       <c r="F14" s="66"/>
     </row>
     <row r="15" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="117"/>
+      <c r="A15" s="118"/>
       <c r="B15" s="18"/>
       <c r="C15" s="72" t="s">
         <v>83</v>
@@ -2540,12 +2808,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A13:A15"/>
     <mergeCell ref="B4:F4"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="A8:A10"/>
-    <mergeCell ref="A13:A15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B12" r:id="rId1"/>
@@ -2601,52 +2869,52 @@
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="122" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="122"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="122" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="125"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="127"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="140" t="s">
+      <c r="A8" s="131" t="s">
         <v>156</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -2666,7 +2934,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="141"/>
+      <c r="A9" s="132"/>
       <c r="B9" s="22" t="s">
         <v>28</v>
       </c>
@@ -2680,7 +2948,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="141"/>
+      <c r="A10" s="132"/>
       <c r="B10" s="5" t="s">
         <v>31</v>
       </c>
@@ -2694,7 +2962,7 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="139"/>
+      <c r="A11" s="116"/>
       <c r="B11" s="15" t="s">
         <v>33</v>
       </c>
@@ -2708,7 +2976,7 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="139"/>
+      <c r="A12" s="116"/>
       <c r="B12" s="15" t="s">
         <v>36</v>
       </c>
@@ -2722,7 +2990,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="139"/>
+      <c r="A13" s="116"/>
       <c r="B13" s="15" t="s">
         <v>38</v>
       </c>
@@ -2736,7 +3004,7 @@
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="139"/>
+      <c r="A14" s="116"/>
       <c r="B14" s="3" t="s">
         <v>40</v>
       </c>
@@ -2762,7 +3030,7 @@
       <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="127" t="s">
+      <c r="A16" s="128" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="15"/>
@@ -2772,7 +3040,7 @@
       <c r="F16" s="13"/>
     </row>
     <row r="17" spans="1:6" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="128"/>
+      <c r="A17" s="129"/>
       <c r="B17" s="26"/>
       <c r="C17" s="28" t="s">
         <v>21</v>
@@ -2784,7 +3052,7 @@
       <c r="F17" s="31"/>
     </row>
     <row r="18" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="128"/>
+      <c r="A18" s="129"/>
       <c r="B18" s="33"/>
       <c r="C18" s="37" t="s">
         <v>44</v>
@@ -2796,7 +3064,7 @@
       <c r="F18" s="35"/>
     </row>
     <row r="19" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="128"/>
+      <c r="A19" s="129"/>
       <c r="B19" s="33"/>
       <c r="C19" s="37" t="s">
         <v>44</v>
@@ -2895,52 +3163,52 @@
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="122" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="122"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="122" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="125"/>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="125"/>
-      <c r="F7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="126"/>
+      <c r="F7" s="127"/>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="118" t="s">
+      <c r="A8" s="119" t="s">
         <v>156</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -2960,7 +3228,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="119"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="22" t="s">
         <v>31</v>
       </c>
@@ -2974,7 +3242,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="130"/>
+      <c r="A10" s="133"/>
       <c r="B10" s="3" t="s">
         <v>33</v>
       </c>
@@ -3000,7 +3268,7 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="128" t="s">
+      <c r="A12" s="129" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="15"/>
@@ -3010,7 +3278,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="335.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="128"/>
+      <c r="A13" s="129"/>
       <c r="B13" s="26"/>
       <c r="C13" s="28" t="s">
         <v>21</v>
@@ -3024,7 +3292,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="57" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="128"/>
+      <c r="A14" s="129"/>
       <c r="B14" s="33"/>
       <c r="C14" s="37" t="s">
         <v>57</v>
@@ -3036,7 +3304,7 @@
       <c r="F14" s="35"/>
     </row>
     <row r="15" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="128"/>
+      <c r="A15" s="129"/>
       <c r="B15" s="33"/>
       <c r="C15" s="37" t="s">
         <v>57</v>
@@ -3048,7 +3316,7 @@
       <c r="F15" s="35"/>
     </row>
     <row r="16" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="128"/>
+      <c r="A16" s="129"/>
       <c r="B16" s="33"/>
       <c r="C16" s="37" t="s">
         <v>60</v>
@@ -3136,52 +3404,52 @@
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="122" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="122"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="122" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="125"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="127"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="132" t="s">
+      <c r="A8" s="135" t="s">
         <v>156</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -3201,7 +3469,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="133"/>
+      <c r="A9" s="136"/>
       <c r="B9" s="22" t="s">
         <v>67</v>
       </c>
@@ -3215,7 +3483,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="133"/>
+      <c r="A10" s="136"/>
       <c r="B10" s="5" t="s">
         <v>70</v>
       </c>
@@ -3229,7 +3497,7 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="134"/>
+      <c r="A11" s="137"/>
       <c r="B11" s="16"/>
       <c r="C11" s="4"/>
       <c r="D11" s="57"/>
@@ -3265,7 +3533,7 @@
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="116" t="s">
+      <c r="A14" s="117" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="15"/>
@@ -3275,7 +3543,7 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="131"/>
+      <c r="A15" s="134"/>
       <c r="B15" s="33"/>
       <c r="C15" s="63" t="s">
         <v>76</v>
@@ -3287,7 +3555,7 @@
       <c r="F15" s="66"/>
     </row>
     <row r="16" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="131"/>
+      <c r="A16" s="134"/>
       <c r="B16" s="35"/>
       <c r="C16" s="67" t="s">
         <v>49</v>
@@ -3299,7 +3567,7 @@
       <c r="F16" s="25"/>
     </row>
     <row r="17" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="131"/>
+      <c r="A17" s="134"/>
       <c r="B17" s="35"/>
       <c r="C17" s="69" t="s">
         <v>79</v>
@@ -3311,7 +3579,7 @@
       <c r="F17" s="31"/>
     </row>
     <row r="18" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="131"/>
+      <c r="A18" s="134"/>
       <c r="B18" s="25"/>
       <c r="C18" s="67" t="s">
         <v>81</v>
@@ -3323,7 +3591,7 @@
       <c r="F18" s="71"/>
     </row>
     <row r="19" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="117"/>
+      <c r="A19" s="118"/>
       <c r="B19" s="18"/>
       <c r="C19" s="72" t="s">
         <v>83</v>
@@ -3397,52 +3665,52 @@
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="122" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="122"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="121" t="s">
+      <c r="B5" s="122" t="s">
         <v>65</v>
       </c>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="123" t="s">
+      <c r="B6" s="124" t="s">
         <v>94</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="125"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="127"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="118" t="s">
+      <c r="A8" s="119" t="s">
         <v>156</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -3462,7 +3730,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="119"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="22" t="s">
         <v>93</v>
       </c>
@@ -3476,7 +3744,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="130"/>
+      <c r="A10" s="133"/>
       <c r="B10" s="39" t="s">
         <v>92</v>
       </c>
@@ -3490,7 +3758,7 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="130"/>
+      <c r="A11" s="133"/>
       <c r="B11" s="56" t="s">
         <v>91</v>
       </c>
@@ -3504,7 +3772,7 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="120"/>
+      <c r="A12" s="121"/>
       <c r="B12" s="57" t="s">
         <v>90</v>
       </c>
@@ -3518,7 +3786,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="120"/>
+      <c r="A13" s="121"/>
       <c r="B13" s="5" t="s">
         <v>89</v>
       </c>
@@ -3568,7 +3836,7 @@
       <c r="F16" s="5"/>
     </row>
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="116" t="s">
+      <c r="A17" s="117" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="15"/>
@@ -3578,7 +3846,7 @@
       <c r="F17" s="5"/>
     </row>
     <row r="18" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="131"/>
+      <c r="A18" s="134"/>
       <c r="B18" s="33"/>
       <c r="C18" s="63" t="s">
         <v>76</v>
@@ -3590,7 +3858,7 @@
       <c r="F18" s="66"/>
     </row>
     <row r="19" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="131"/>
+      <c r="A19" s="134"/>
       <c r="B19" s="35"/>
       <c r="C19" s="67" t="s">
         <v>76</v>
@@ -3602,7 +3870,7 @@
       <c r="F19" s="25"/>
     </row>
     <row r="20" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="131"/>
+      <c r="A20" s="134"/>
       <c r="B20" s="35"/>
       <c r="C20" s="69" t="s">
         <v>79</v>
@@ -3614,7 +3882,7 @@
       <c r="F20" s="31"/>
     </row>
     <row r="21" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="131"/>
+      <c r="A21" s="134"/>
       <c r="B21" s="25"/>
       <c r="C21" s="67" t="s">
         <v>81</v>
@@ -3626,7 +3894,7 @@
       <c r="F21" s="71"/>
     </row>
     <row r="22" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="117"/>
+      <c r="A22" s="118"/>
       <c r="B22" s="18"/>
       <c r="C22" s="72" t="s">
         <v>49</v>
@@ -3654,6 +3922,215 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="59.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2">
+        <v>43575</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="122" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="123"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="122" t="s">
+        <v>163</v>
+      </c>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="123"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="124" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="125"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="126" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="127"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="135" t="s">
+        <v>159</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="136"/>
+      <c r="B9" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="54" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="55">
+        <v>1</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="136"/>
+      <c r="B10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="56">
+        <v>2</v>
+      </c>
+      <c r="E10" s="55"/>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="137"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="57"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="117" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="142"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="64" t="s">
+        <v>160</v>
+      </c>
+      <c r="E14" s="65"/>
+      <c r="F14" s="66"/>
+    </row>
+    <row r="15" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="143"/>
+      <c r="B15" s="80"/>
+      <c r="C15" s="67" t="s">
+        <v>161</v>
+      </c>
+      <c r="D15" s="68" t="s">
+        <v>162</v>
+      </c>
+      <c r="E15" s="30"/>
+      <c r="F15" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A13:A15"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B12" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
@@ -3700,52 +4177,52 @@
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="139" t="s">
         <v>105</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="122"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="135" t="s">
+      <c r="B5" s="139" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="136" t="s">
+      <c r="B6" s="140" t="s">
         <v>97</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="125"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="127"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="118" t="s">
+      <c r="A8" s="119" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -3765,7 +4242,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="119"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="84" t="s">
         <v>98</v>
       </c>
@@ -3815,7 +4292,7 @@
       <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="116" t="s">
+      <c r="A13" s="117" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="15"/>
@@ -3825,7 +4302,7 @@
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="135" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="131"/>
+      <c r="A14" s="134"/>
       <c r="B14" s="33"/>
       <c r="C14" s="87" t="s">
         <v>76</v>
@@ -3837,7 +4314,7 @@
       <c r="F14" s="66"/>
     </row>
     <row r="15" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="131"/>
+      <c r="A15" s="134"/>
       <c r="B15" s="35"/>
       <c r="C15" s="90" t="s">
         <v>62</v>
@@ -3877,7 +4354,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F16"/>
   <sheetViews>
@@ -3924,52 +4401,52 @@
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="139" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="122"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="135" t="s">
+      <c r="B5" s="139" t="s">
         <v>107</v>
       </c>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="136" t="s">
+      <c r="B6" s="140" t="s">
         <v>104</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="125"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="137" t="s">
+      <c r="B7" s="141" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="127"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="118" t="s">
+      <c r="A8" s="119" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -3989,7 +4466,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="119"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="84" t="s">
         <v>103</v>
       </c>
@@ -4003,7 +4480,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="130"/>
+      <c r="A10" s="133"/>
       <c r="B10" s="93" t="s">
         <v>108</v>
       </c>
@@ -4055,7 +4532,7 @@
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="116" t="s">
+      <c r="A14" s="117" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="15"/>
@@ -4065,7 +4542,7 @@
       <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:6" ht="235.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="131"/>
+      <c r="A15" s="134"/>
       <c r="B15" s="33"/>
       <c r="C15" s="63" t="s">
         <v>76</v>
@@ -4104,7 +4581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F24"/>
   <sheetViews>
@@ -4151,52 +4628,52 @@
       <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="135" t="s">
+      <c r="B4" s="139" t="s">
         <v>113</v>
       </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="122"/>
+      <c r="C4" s="122"/>
+      <c r="D4" s="122"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="123"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="135" t="s">
+      <c r="B5" s="139" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="122"/>
+      <c r="C5" s="122"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="122"/>
+      <c r="F5" s="123"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="136" t="s">
+      <c r="B6" s="140" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="124"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
+      <c r="F6" s="125"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="125" t="s">
+      <c r="B7" s="126" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="126"/>
+      <c r="C7" s="126"/>
+      <c r="D7" s="126"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="127"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="118" t="s">
+      <c r="A8" s="119" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -4216,7 +4693,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="119"/>
+      <c r="A9" s="120"/>
       <c r="B9" s="84" t="s">
         <v>28</v>
       </c>
@@ -4232,7 +4709,7 @@
       <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="130"/>
+      <c r="A10" s="133"/>
       <c r="B10" s="93" t="s">
         <v>36</v>
       </c>
@@ -4248,7 +4725,7 @@
       <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="130"/>
+      <c r="A11" s="133"/>
       <c r="B11" s="94" t="s">
         <v>115</v>
       </c>
@@ -4264,7 +4741,7 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="120"/>
+      <c r="A12" s="121"/>
       <c r="B12" s="102" t="s">
         <v>38</v>
       </c>
@@ -4280,7 +4757,7 @@
       <c r="F12" s="83"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="130"/>
+      <c r="A13" s="133"/>
       <c r="B13" s="105" t="s">
         <v>117</v>
       </c>
@@ -4296,7 +4773,7 @@
       <c r="F13" s="106"/>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="130"/>
+      <c r="A14" s="133"/>
       <c r="B14" s="105" t="s">
         <v>119</v>
       </c>
@@ -4312,7 +4789,7 @@
       <c r="F14" s="110"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="130"/>
+      <c r="A15" s="133"/>
       <c r="B15" s="105" t="s">
         <v>121</v>
       </c>
@@ -4328,7 +4805,7 @@
       <c r="F15" s="110"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="130"/>
+      <c r="A16" s="133"/>
       <c r="B16" s="105" t="s">
         <v>122</v>
       </c>
@@ -4344,7 +4821,7 @@
       <c r="F16" s="110"/>
     </row>
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="120"/>
+      <c r="A17" s="121"/>
       <c r="B17" s="101" t="s">
         <v>123</v>
       </c>
@@ -4396,7 +4873,7 @@
       <c r="F20" s="5"/>
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="116" t="s">
+      <c r="A21" s="117" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="15"/>
@@ -4406,7 +4883,7 @@
       <c r="F21" s="5"/>
     </row>
     <row r="22" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="131"/>
+      <c r="A22" s="134"/>
       <c r="B22" s="33"/>
       <c r="C22" s="63" t="s">
         <v>76</v>
@@ -4418,7 +4895,7 @@
       <c r="F22" s="66"/>
     </row>
     <row r="23" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="131"/>
+      <c r="A23" s="134"/>
       <c r="B23" s="113"/>
       <c r="C23" s="90" t="s">
         <v>83</v>
@@ -4430,7 +4907,7 @@
       <c r="F23" s="25"/>
     </row>
     <row r="24" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="117"/>
+      <c r="A24" s="118"/>
       <c r="B24" s="18"/>
       <c r="C24" s="72" t="s">
         <v>49</v>
@@ -4455,241 +4932,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="59.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5703125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2">
-        <v>43575</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="135" t="s">
-        <v>129</v>
-      </c>
-      <c r="C4" s="121"/>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="122"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="135" t="s">
-        <v>130</v>
-      </c>
-      <c r="C5" s="121"/>
-      <c r="D5" s="121"/>
-      <c r="E5" s="121"/>
-      <c r="F5" s="122"/>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="136" t="s">
-        <v>131</v>
-      </c>
-      <c r="C6" s="123"/>
-      <c r="D6" s="123"/>
-      <c r="E6" s="123"/>
-      <c r="F6" s="124"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="125" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="125"/>
-      <c r="D7" s="125"/>
-      <c r="E7" s="129"/>
-      <c r="F7" s="126"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="118" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="53" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="44" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="119"/>
-      <c r="B9" s="84" t="s">
-        <v>134</v>
-      </c>
-      <c r="C9" s="86" t="s">
-        <v>133</v>
-      </c>
-      <c r="D9" s="86">
-        <v>10.8770936</v>
-      </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="130"/>
-      <c r="B10" s="93" t="s">
-        <v>132</v>
-      </c>
-      <c r="C10" s="100" t="s">
-        <v>133</v>
-      </c>
-      <c r="D10" s="105">
-        <v>106.8032315</v>
-      </c>
-      <c r="E10" s="86"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="75"/>
-      <c r="B11" s="16"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="111"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="60" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12" s="77" t="s">
-        <v>73</v>
-      </c>
-      <c r="D12" s="61" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="17" t="s">
-        <v>135</v>
-      </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="116" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="131"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="63" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="88" t="s">
-        <v>137</v>
-      </c>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
-    </row>
-    <row r="16" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="131"/>
-      <c r="B16" s="113"/>
-      <c r="C16" s="90" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" s="89" t="s">
-        <v>136</v>
-      </c>
-      <c r="E16" s="30"/>
-      <c r="F16" s="25"/>
-    </row>
-    <row r="17" spans="1:6" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="117"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="72" t="s">
-        <v>49</v>
-      </c>
-      <c r="D17" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="E17" s="73"/>
-      <c r="F17" s="74"/>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="A8:A10"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>